<commit_message>
entered data and updated meta tabs
</commit_message>
<xml_diff>
--- a/data/Buds Sheet.xlsx
+++ b/data/Buds Sheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="3360" windowWidth="28400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="22800" yWindow="460" windowWidth="28400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="meta" sheetId="2" r:id="rId1"/>
+    <sheet name="observations" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="202">
   <si>
     <t>NEW</t>
   </si>
@@ -486,13 +487,160 @@
   </si>
   <si>
     <t>/, 9, 9, /, /, /</t>
+  </si>
+  <si>
+    <t>Cells in green have been put in the growth chamber</t>
+  </si>
+  <si>
+    <t>cells that are blue were watered that day</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Growth Chamber</t>
+  </si>
+  <si>
+    <t>Growth Chamber: -3degC, light ~280 for 12 hrs</t>
+  </si>
+  <si>
+    <t>Put in for 18-30 hrs depending on time line - aim for 24 hrs</t>
+  </si>
+  <si>
+    <t>TABS</t>
+  </si>
+  <si>
+    <t>BBCH observations for all individuals through leaf out, once the individual is past leaf out then they were no longer monitored</t>
+  </si>
+  <si>
+    <t>observations</t>
+  </si>
+  <si>
+    <t>observations tab:</t>
+  </si>
+  <si>
+    <t>ID number created for experiment</t>
+  </si>
+  <si>
+    <t>A or B - control or false spring</t>
+  </si>
+  <si>
+    <t>what color bud is it?</t>
+  </si>
+  <si>
+    <t>Blue, Red, Green, Black - are all marker colors</t>
+  </si>
+  <si>
+    <t>Yellow, White, Blue, Green, Red, Black and any variation are all tags</t>
+  </si>
+  <si>
+    <t>ex. Y-B,R,G,B means Yellow tag branch, Blue marker bud, Red marker bud, Green marker bud, and black marker bud</t>
+  </si>
+  <si>
+    <t>BU = blue</t>
+  </si>
+  <si>
+    <t>BA = black</t>
+  </si>
+  <si>
+    <t>ex. R/Y - red and yellow tagged bud</t>
+  </si>
+  <si>
+    <t>ex. 9,/,10,11 - corresponds to list under bud column</t>
+  </si>
+  <si>
+    <t>labeled as 9-15</t>
+  </si>
+  <si>
+    <t>can also have notes about discoloration or wilting after false spring treatment</t>
+  </si>
+  <si>
+    <t>Moved to GH 10 on Mar 24, 2017</t>
+  </si>
+  <si>
+    <t>GH:</t>
+  </si>
+  <si>
+    <t>humM</t>
+  </si>
+  <si>
+    <t>humL</t>
+  </si>
+  <si>
+    <t>humH</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>tempL</t>
+  </si>
+  <si>
+    <t>tempH</t>
+  </si>
+  <si>
+    <t>tempM</t>
+  </si>
+  <si>
+    <t>From GH 7: (actually more ambient conditions, similar to outdoors, these values are from one recording)</t>
+  </si>
+  <si>
+    <t>Marked all buds on April 4-5 and started monitoring budburst then. Go about 3-4 times a week to monitor</t>
+  </si>
+  <si>
+    <t>BBCH 13.04</t>
+  </si>
+  <si>
+    <t>9,/,15,15,15</t>
+  </si>
+  <si>
+    <t>9,/,/</t>
+  </si>
+  <si>
+    <t>9,9,10</t>
+  </si>
+  <si>
+    <t>/,/,9</t>
+  </si>
+  <si>
+    <t>11,10,10</t>
+  </si>
+  <si>
+    <t>15,12,14,11,11</t>
+  </si>
+  <si>
+    <t>9,/</t>
+  </si>
+  <si>
+    <t>9,/,/,/</t>
+  </si>
+  <si>
+    <t>9,9,9,/</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>9,9,/,/</t>
+  </si>
+  <si>
+    <t>9,9,/,/,/</t>
+  </si>
+  <si>
+    <t>9,/,/,/,/</t>
+  </si>
+  <si>
+    <t>BBCH 11.4 (post-frz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -520,6 +668,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -541,12 +696,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,10 +980,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G372"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="E367" sqref="E367"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H372"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A171" sqref="A171:B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,9 +1254,10 @@
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,13 +1274,16 @@
         <v>146</v>
       </c>
       <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -877,31 +1299,37 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>54</v>
       </c>
       <c r="E3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -917,8 +1345,11 @@
       <c r="E7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>54</v>
       </c>
@@ -928,18 +1359,21 @@
       <c r="E8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -950,43 +1384,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="C13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="C14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="C15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="C17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1002,8 +1436,11 @@
       <c r="E18">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="C19" t="s">
         <v>54</v>
@@ -1014,26 +1451,29 @@
       <c r="E19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="C22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1044,31 +1484,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="C24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="C27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1084,8 +1524,11 @@
       <c r="E28">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="C29" t="s">
         <v>54</v>
@@ -1093,8 +1536,11 @@
       <c r="E29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="C30" t="s">
         <v>56</v>
@@ -1105,8 +1551,11 @@
       <c r="E30">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="C31" t="s">
         <v>57</v>
@@ -1114,8 +1563,11 @@
       <c r="E31">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="C32" t="s">
         <v>58</v>
@@ -1126,8 +1578,11 @@
       <c r="E32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="C33" t="s">
         <v>59</v>
@@ -1138,8 +1593,11 @@
       <c r="E33">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1155,8 +1613,11 @@
       <c r="E34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="C35" t="s">
         <v>54</v>
@@ -1167,20 +1628,26 @@
       <c r="E35">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="C36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="C37" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="C38" t="s">
         <v>58</v>
@@ -1191,8 +1658,11 @@
       <c r="E38">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
         <v>59</v>
@@ -1203,14 +1673,17 @@
       <c r="E39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1224,7 +1697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="C42" t="s">
         <v>54</v>
@@ -1233,7 +1706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="C43" t="s">
         <v>56</v>
@@ -1242,25 +1715,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="C44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="C45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="C46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -1276,8 +1749,11 @@
       <c r="E47">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="C48" t="s">
         <v>54</v>
@@ -1288,8 +1764,11 @@
       <c r="E48">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="C49" t="s">
         <v>56</v>
@@ -1300,8 +1779,11 @@
       <c r="E49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="C50" t="s">
         <v>57</v>
@@ -1309,8 +1791,11 @@
       <c r="E50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="C51" t="s">
         <v>58</v>
@@ -1318,20 +1803,23 @@
       <c r="E51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="C52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="C53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -1347,32 +1835,38 @@
       <c r="E54">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="C55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="C56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="C57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="C58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="C59" t="s">
         <v>59</v>
@@ -1383,8 +1877,11 @@
       <c r="E59">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="C60" t="s">
         <v>55</v>
@@ -1395,12 +1892,15 @@
       <c r="E60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="G60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C61" t="s">
@@ -1412,21 +1912,27 @@
       <c r="E61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="F61">
+        <v>11</v>
+      </c>
+      <c r="G61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="4">
         <v>42835</v>
       </c>
       <c r="C62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="4">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="5">
         <v>0.40069444444444446</v>
       </c>
       <c r="C63" t="s">
@@ -1438,26 +1944,32 @@
       <c r="E63">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>12</v>
+      </c>
+      <c r="G63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="C64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="C65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="C66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>15</v>
       </c>
@@ -1473,48 +1985,54 @@
       <c r="E67">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="C68" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="C69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="C70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="C71" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="C72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="C73" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+      <c r="G73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C74" t="s">
@@ -1526,12 +2044,18 @@
       <c r="E74">
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="F74">
+        <v>11</v>
+      </c>
+      <c r="G74">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="4">
         <v>42835</v>
       </c>
       <c r="C75" t="s">
@@ -1543,10 +2067,16 @@
       <c r="E75">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-      <c r="B76" s="4">
+      <c r="F75">
+        <v>9</v>
+      </c>
+      <c r="G75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="5">
         <v>0.40069444444444446</v>
       </c>
       <c r="C76" t="s">
@@ -1558,26 +2088,32 @@
       <c r="E76">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>10</v>
+      </c>
+      <c r="G76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="C77" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="C78" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="C79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -1593,8 +2129,11 @@
       <c r="E80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="C81" t="s">
         <v>59</v>
@@ -1602,14 +2141,20 @@
       <c r="E81">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="C82" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>18</v>
       </c>
@@ -1625,14 +2170,17 @@
       <c r="E83">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="C84" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="C85" t="s">
         <v>56</v>
@@ -1643,32 +2191,35 @@
       <c r="E85">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="C86" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="C87" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="C88" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="C89" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>19</v>
       </c>
@@ -1684,32 +2235,35 @@
       <c r="E90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="C91" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="C92" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="C93" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="C94" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>20</v>
       </c>
@@ -1725,8 +2279,11 @@
       <c r="E95">
         <v>10</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="C96" t="s">
         <v>54</v>
@@ -2151,19 +2708,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="C161" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="C162" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>28</v>
       </c>
@@ -2174,53 +2731,53 @@
         <v>55</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="C164" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="C165" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="C166" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="C167" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="C168" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="C169" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="C170" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C171" t="s">
@@ -2232,12 +2789,18 @@
       <c r="E171">
         <v>12</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
+      <c r="F171">
+        <v>12</v>
+      </c>
+      <c r="G171">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B172" s="3">
+      <c r="B172" s="4">
         <v>42835</v>
       </c>
       <c r="C172" t="s">
@@ -2249,10 +2812,16 @@
       <c r="E172">
         <v>9</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="1"/>
-      <c r="B173" s="4">
+      <c r="F172">
+        <v>9</v>
+      </c>
+      <c r="G172">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="3"/>
+      <c r="B173" s="5">
         <v>0.40069444444444446</v>
       </c>
       <c r="C173" t="s">
@@ -2264,8 +2833,14 @@
       <c r="E173">
         <v>12</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173">
+        <v>12</v>
+      </c>
+      <c r="G173">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="C174" t="s">
         <v>57</v>
@@ -2276,8 +2851,14 @@
       <c r="E174">
         <v>11</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174">
+        <v>11</v>
+      </c>
+      <c r="G174">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="C175" t="s">
         <v>93</v>
@@ -2288,8 +2869,14 @@
       <c r="E175" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175" t="s">
+        <v>187</v>
+      </c>
+      <c r="G175" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>30</v>
       </c>
@@ -2613,25 +3200,28 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="C225" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="C226" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G226" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="C227" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>36</v>
       </c>
@@ -2642,49 +3232,49 @@
         <v>55</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="C229" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="C230" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="C231" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="C232" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="C233" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="C234" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="C235" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="C236" t="s">
         <v>70</v>
@@ -2693,13 +3283,13 @@
         <v>149</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="C237" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>37</v>
       </c>
@@ -2710,43 +3300,49 @@
         <v>55</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="C239" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="C240" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="C241" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="C242" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="C243" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G243" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="C244" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G244" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="C245" t="s">
         <v>75</v>
@@ -2757,14 +3353,17 @@
       <c r="E245" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G245" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="C246" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="C247" t="s">
         <v>114</v>
@@ -2775,8 +3374,11 @@
       <c r="E247" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G247" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>38</v>
       </c>
@@ -2787,67 +3389,82 @@
         <v>55</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="C249" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="C250" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="C251" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="C252" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="C253" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G253" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="C254" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="C255" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G255" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="C256" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G256" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="C257" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G257" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="C258" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G258" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="C259" t="s">
         <v>116</v>
@@ -2858,8 +3475,11 @@
       <c r="E259" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G259" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="C260" t="s">
         <v>117</v>
@@ -2870,8 +3490,11 @@
       <c r="E260" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G260" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>39</v>
       </c>
@@ -2882,31 +3505,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1"/>
       <c r="C262" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="C263" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="C264" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="C265" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>40</v>
       </c>
@@ -2917,67 +3540,67 @@
         <v>55</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="1"/>
       <c r="C267" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="C268" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="C269" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="C270" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="C271" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="C272" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="C273" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="C274" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="C275" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="C276" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>41</v>
       </c>
@@ -2988,61 +3611,64 @@
         <v>55</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="C278" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="C279" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="C280" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="C281" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="1"/>
       <c r="C282" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="C283" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="1"/>
       <c r="C284" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="1"/>
       <c r="C285" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="1"/>
       <c r="C286" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G286">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="C287" t="s">
         <v>83</v>
@@ -3050,8 +3676,11 @@
       <c r="E287" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G287" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>42</v>
       </c>
@@ -3061,74 +3690,92 @@
       <c r="C288" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G288">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="1"/>
       <c r="C289" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="C290" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="C291" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="C292" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="C293" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G293" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="C294" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G294" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="C295" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G295" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="C296" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="C297" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G297" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="C298" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G298" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="C299" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>43</v>
       </c>
@@ -3139,25 +3786,25 @@
         <v>55</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="C301" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="C302" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="C303" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="C304" t="s">
         <v>123</v>
@@ -3375,67 +4022,73 @@
         <v>57</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" s="1"/>
       <c r="C337" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="C338" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="C339" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="C340" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" s="1"/>
       <c r="C341" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" s="1"/>
       <c r="C342" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G342" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" s="1"/>
       <c r="C343" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" s="1"/>
       <c r="C344" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" s="1"/>
       <c r="C345" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="C346" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G346" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>48</v>
       </c>
@@ -3446,31 +4099,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="C348" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
       <c r="C349" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="C350" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" s="1"/>
       <c r="C351" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>49</v>
       </c>
@@ -3481,43 +4134,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="C353" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="C354" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="C355" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="C356" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="C357" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="C358" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>50</v>
       </c>
@@ -3528,43 +4181,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="C360" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A361" s="1"/>
       <c r="C361" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="C362" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="C363" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="C364" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="C365" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>51</v>
       </c>
@@ -3577,13 +4230,16 @@
       <c r="E366">
         <v>9</v>
       </c>
-    </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G366">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C367" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C368" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
updates to bbch data for both exps
</commit_message>
<xml_diff>
--- a/data/Buds Sheet.xlsx
+++ b/data/Buds Sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22800" yWindow="460" windowWidth="28400" windowHeight="21160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8400" yWindow="1900" windowWidth="28400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="271">
   <si>
     <t>NEW</t>
   </si>
@@ -634,6 +634,213 @@
   </si>
   <si>
     <t>BBCH 11.4 (post-frz)</t>
+  </si>
+  <si>
+    <t>BBCH 17.04</t>
+  </si>
+  <si>
+    <t>9,9,9,9,9,9</t>
+  </si>
+  <si>
+    <t>9,9,9</t>
+  </si>
+  <si>
+    <t>10,9,/,/</t>
+  </si>
+  <si>
+    <t>10,10,9,9</t>
+  </si>
+  <si>
+    <t>14,10,9</t>
+  </si>
+  <si>
+    <t>11,11,9</t>
+  </si>
+  <si>
+    <t>UNFRZ</t>
+  </si>
+  <si>
+    <t>Looks great!</t>
+  </si>
+  <si>
+    <t>10,9,9,10,/,/</t>
+  </si>
+  <si>
+    <t>14,13,15</t>
+  </si>
+  <si>
+    <t>9,/,11</t>
+  </si>
+  <si>
+    <t>15,14,14</t>
+  </si>
+  <si>
+    <t>10,9,9,9,10,9</t>
+  </si>
+  <si>
+    <t>15,9,14,15,15,15,15</t>
+  </si>
+  <si>
+    <t>10,/</t>
+  </si>
+  <si>
+    <t>10,/,/,/</t>
+  </si>
+  <si>
+    <t>10,9,9</t>
+  </si>
+  <si>
+    <t>12,11,11,10</t>
+  </si>
+  <si>
+    <t>10,9,10,9</t>
+  </si>
+  <si>
+    <t>15,15</t>
+  </si>
+  <si>
+    <t>10,12</t>
+  </si>
+  <si>
+    <t>10,14,12,10</t>
+  </si>
+  <si>
+    <t>/,9,/</t>
+  </si>
+  <si>
+    <t>/,/,/,9,9</t>
+  </si>
+  <si>
+    <t>9,9,9,9</t>
+  </si>
+  <si>
+    <t>/,10</t>
+  </si>
+  <si>
+    <t>/,10,10,9</t>
+  </si>
+  <si>
+    <t>15,14,12,12</t>
+  </si>
+  <si>
+    <t>10,/,9,9</t>
+  </si>
+  <si>
+    <t>9,9</t>
+  </si>
+  <si>
+    <t>10,11,10,9</t>
+  </si>
+  <si>
+    <t>BBCH 24.04</t>
+  </si>
+  <si>
+    <t>9,/,9</t>
+  </si>
+  <si>
+    <t>13,14,9,10</t>
+  </si>
+  <si>
+    <t>15,14,13</t>
+  </si>
+  <si>
+    <t>15,15,13</t>
+  </si>
+  <si>
+    <t>15,14,15,14,/,/</t>
+  </si>
+  <si>
+    <t>15,15,15</t>
+  </si>
+  <si>
+    <t>13,/,14</t>
+  </si>
+  <si>
+    <t>14,14,14,15,13</t>
+  </si>
+  <si>
+    <t>15,15,15,15,15</t>
+  </si>
+  <si>
+    <t>9,10,/</t>
+  </si>
+  <si>
+    <t>13,12</t>
+  </si>
+  <si>
+    <t>13,15,14</t>
+  </si>
+  <si>
+    <t>15,15,15,14</t>
+  </si>
+  <si>
+    <t>14,15,15,15</t>
+  </si>
+  <si>
+    <t>10,10,11,9</t>
+  </si>
+  <si>
+    <t>15,15,14,11</t>
+  </si>
+  <si>
+    <t>10,9,9,9</t>
+  </si>
+  <si>
+    <t>9,9,9,/,/</t>
+  </si>
+  <si>
+    <t>10,/,9,/,/</t>
+  </si>
+  <si>
+    <t>10,9,12,12,12</t>
+  </si>
+  <si>
+    <t>13,12,12,9</t>
+  </si>
+  <si>
+    <t>/,11,13</t>
+  </si>
+  <si>
+    <t>/,15</t>
+  </si>
+  <si>
+    <t>/,9,11</t>
+  </si>
+  <si>
+    <t>14,15</t>
+  </si>
+  <si>
+    <t>12,11</t>
+  </si>
+  <si>
+    <t>/,/,10,9,9</t>
+  </si>
+  <si>
+    <t>/,/,/,/,9</t>
+  </si>
+  <si>
+    <t>9,15,/,14</t>
+  </si>
+  <si>
+    <t>11,15,15,15,15</t>
+  </si>
+  <si>
+    <t>11,10</t>
+  </si>
+  <si>
+    <t>14,/,13,11,11</t>
+  </si>
+  <si>
+    <t>14,13,12</t>
+  </si>
+  <si>
+    <t>13,13</t>
+  </si>
+  <si>
+    <t>9,10,10</t>
+  </si>
+  <si>
+    <t>15,15,15,15</t>
   </si>
 </sst>
 </file>
@@ -1242,22 +1449,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H372"/>
+  <dimension ref="A1:K372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A171" sqref="A171:B173"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C183" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="14" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1280,10 +1493,19 @@
         <v>186</v>
       </c>
       <c r="H1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1302,8 +1524,14 @@
       <c r="G2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>54</v>
       </c>
@@ -1313,23 +1541,38 @@
       <c r="G3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1348,8 +1591,14 @@
       <c r="G7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>54</v>
       </c>
@@ -1362,18 +1611,24 @@
       <c r="G8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1384,43 +1639,55 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="C13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="C14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="C15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="C17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1439,8 +1706,14 @@
       <c r="G18">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="C19" t="s">
         <v>54</v>
@@ -1454,26 +1727,32 @@
       <c r="G19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="C22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1484,31 +1763,37 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="C24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>9</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="C27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1527,8 +1812,14 @@
       <c r="G28">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="C29" t="s">
         <v>54</v>
@@ -1539,8 +1830,14 @@
       <c r="G29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="C30" t="s">
         <v>56</v>
@@ -1554,8 +1851,14 @@
       <c r="G30">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>14</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="C31" t="s">
         <v>57</v>
@@ -1566,8 +1869,14 @@
       <c r="G31">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="C32" t="s">
         <v>58</v>
@@ -1581,8 +1890,14 @@
       <c r="G32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>12</v>
+      </c>
+      <c r="I32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="C33" t="s">
         <v>59</v>
@@ -1596,8 +1911,14 @@
       <c r="G33">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>11</v>
+      </c>
+      <c r="I33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1616,8 +1937,14 @@
       <c r="G34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="C35" t="s">
         <v>54</v>
@@ -1631,14 +1958,23 @@
       <c r="G35">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>11</v>
+      </c>
+      <c r="I35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="C36" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="C37" t="s">
         <v>57</v>
@@ -1646,8 +1982,14 @@
       <c r="G37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="C38" t="s">
         <v>58</v>
@@ -1661,8 +2003,14 @@
       <c r="G38">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>9</v>
+      </c>
+      <c r="I38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
         <v>59</v>
@@ -1676,14 +2024,20 @@
       <c r="G39">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>14</v>
+      </c>
+      <c r="I39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1696,8 +2050,14 @@
       <c r="E41">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="C42" t="s">
         <v>54</v>
@@ -1705,8 +2065,14 @@
       <c r="E42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>9</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="C43" t="s">
         <v>56</v>
@@ -1714,26 +2080,38 @@
       <c r="E43">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>9</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="C44" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>9</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="C45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="C46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -1752,8 +2130,14 @@
       <c r="G47">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="C48" t="s">
         <v>54</v>
@@ -1767,8 +2151,14 @@
       <c r="G48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>10</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="C49" t="s">
         <v>56</v>
@@ -1782,8 +2172,14 @@
       <c r="G49">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>11</v>
+      </c>
+      <c r="I49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="C50" t="s">
         <v>57</v>
@@ -1794,8 +2190,14 @@
       <c r="G50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>9</v>
+      </c>
+      <c r="I50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="C51" t="s">
         <v>58</v>
@@ -1806,20 +2208,26 @@
       <c r="G51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>9</v>
+      </c>
+      <c r="I51">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="C52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="C53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -1838,20 +2246,35 @@
       <c r="G54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>10</v>
+      </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="C55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="C56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>11</v>
+      </c>
+      <c r="I56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="C57" t="s">
         <v>57</v>
@@ -1859,14 +2282,20 @@
       <c r="G57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>11</v>
+      </c>
+      <c r="I57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="C58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="C59" t="s">
         <v>59</v>
@@ -1880,8 +2309,14 @@
       <c r="G59">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>10</v>
+      </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="C60" t="s">
         <v>55</v>
@@ -1895,8 +2330,14 @@
       <c r="G60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>10</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>14</v>
       </c>
@@ -1918,8 +2359,14 @@
       <c r="G61">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <v>15</v>
+      </c>
+      <c r="I61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>147</v>
       </c>
@@ -1929,8 +2376,14 @@
       <c r="C62" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>10</v>
+      </c>
+      <c r="I62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="5">
         <v>0.40069444444444446</v>
@@ -1950,26 +2403,45 @@
       <c r="G63">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="H63">
+        <v>14</v>
+      </c>
+      <c r="I63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="4">
+        <v>42836</v>
+      </c>
       <c r="C64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="5">
+        <v>0.43333333333333335</v>
+      </c>
       <c r="C65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>42849</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="C66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>15</v>
       </c>
@@ -1988,38 +2460,62 @@
       <c r="G67">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="C68" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="C69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="C70" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>9</v>
+      </c>
+      <c r="I70">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="C71" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>9</v>
+      </c>
+      <c r="I71">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="C72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>9</v>
+      </c>
+      <c r="I72">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="C73" t="s">
         <v>55</v>
@@ -2027,8 +2523,14 @@
       <c r="G73">
         <v>11</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>13</v>
+      </c>
+      <c r="I73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
@@ -2050,8 +2552,14 @@
       <c r="G74">
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>11</v>
+      </c>
+      <c r="I74">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>147</v>
       </c>
@@ -2073,8 +2581,14 @@
       <c r="G75">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>10</v>
+      </c>
+      <c r="I75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="5">
         <v>0.40069444444444446</v>
@@ -2094,26 +2608,46 @@
       <c r="G76">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
+      <c r="H76">
+        <v>10</v>
+      </c>
+      <c r="I76">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" s="4">
+        <v>42836</v>
+      </c>
       <c r="C77" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="5">
+        <v>0.43333333333333335</v>
+      </c>
       <c r="C78" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>9</v>
+      </c>
+      <c r="I78">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="C79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2132,9 +2666,20 @@
       <c r="G80">
         <v>11</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="1"/>
+      <c r="H80">
+        <v>13</v>
+      </c>
+      <c r="I80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>42842</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0.3576388888888889</v>
+      </c>
       <c r="C81" t="s">
         <v>59</v>
       </c>
@@ -2144,17 +2689,31 @@
       <c r="G81">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="1"/>
+      <c r="H81">
+        <v>9</v>
+      </c>
+      <c r="I81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>42843</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0.3298611111111111</v>
+      </c>
       <c r="C82" t="s">
         <v>55</v>
       </c>
       <c r="G82">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>18</v>
       </c>
@@ -2173,14 +2732,17 @@
       <c r="G83">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="C84" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="C85" t="s">
         <v>56</v>
@@ -2194,32 +2756,53 @@
       <c r="G85">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>9</v>
+      </c>
+      <c r="I85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="C86" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>9</v>
+      </c>
+      <c r="I86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="C87" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>9</v>
+      </c>
+      <c r="I87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="C88" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="C89" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>19</v>
       </c>
@@ -2238,32 +2821,44 @@
       <c r="G90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>10</v>
+      </c>
+      <c r="I90">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="C91" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <v>9</v>
+      </c>
+      <c r="I91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="C92" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="C93" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="C94" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>20</v>
       </c>
@@ -2282,38 +2877,56 @@
       <c r="G95">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>9</v>
+      </c>
+      <c r="I95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="C96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="C97" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I97">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="C98" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="C99" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="C100" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>21</v>
       </c>
@@ -2324,31 +2937,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="C102" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="C103" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="C104" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="C105" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>22</v>
       </c>
@@ -2359,37 +2972,37 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="C107" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="C108" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="C109" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="C110" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="C111" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="C112" t="s">
         <v>62</v>
@@ -2602,19 +3215,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="C145" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="C146" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>26</v>
       </c>
@@ -2624,50 +3237,56 @@
       <c r="C147" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H147">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="C148" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="C149" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="C150" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="C151" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H151" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="C152" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="C153" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="C154" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>27</v>
       </c>
@@ -2678,49 +3297,49 @@
         <v>55</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="C156" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="C157" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="C158" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="C159" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="C160" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="C161" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="C162" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>28</v>
       </c>
@@ -2731,49 +3350,49 @@
         <v>55</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="C164" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="C165" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="C166" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="C167" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="C168" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="C169" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="C170" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>29</v>
       </c>
@@ -2795,13 +3414,16 @@
       <c r="G171">
         <v>14</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A172" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B172" s="4">
+      <c r="H171">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="4">
         <v>42835</v>
+      </c>
+      <c r="B172" s="5">
+        <v>0.40069444444444446</v>
       </c>
       <c r="C172" t="s">
         <v>54</v>
@@ -2818,11 +3440,16 @@
       <c r="G172">
         <v>9</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="3"/>
+      <c r="H172">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" s="4">
+        <v>42836</v>
+      </c>
       <c r="B173" s="5">
-        <v>0.40069444444444446</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="C173" t="s">
         <v>56</v>
@@ -2839,9 +3466,17 @@
       <c r="G173">
         <v>14</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A174" s="1"/>
+      <c r="H173">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="4">
+        <v>42842</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>210</v>
+      </c>
       <c r="C174" t="s">
         <v>57</v>
       </c>
@@ -2857,9 +3492,13 @@
       <c r="G174">
         <v>12</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A175" s="1"/>
+      <c r="H174">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" s="3"/>
+      <c r="B175" s="5"/>
       <c r="C175" t="s">
         <v>93</v>
       </c>
@@ -2875,8 +3514,11 @@
       <c r="G175" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H175" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>30</v>
       </c>
@@ -3200,13 +3842,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="C225" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="C226" t="s">
         <v>106</v>
@@ -3214,14 +3856,26 @@
       <c r="G226" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H226" t="s">
+        <v>188</v>
+      </c>
+      <c r="I226" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="C227" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H227" t="s">
+        <v>203</v>
+      </c>
+      <c r="I227" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>36</v>
       </c>
@@ -3231,50 +3885,86 @@
       <c r="C228" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I228">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="C229" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I229">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="C230" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I230">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="C231" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I231">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="C232" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H232" t="s">
+        <v>204</v>
+      </c>
+      <c r="I232" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="C233" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H233" t="s">
+        <v>198</v>
+      </c>
+      <c r="I233" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="C234" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H234" t="s">
+        <v>205</v>
+      </c>
+      <c r="I234" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="C235" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H235" t="s">
+        <v>206</v>
+      </c>
+      <c r="I235" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="C236" t="s">
         <v>70</v>
@@ -3282,14 +3972,26 @@
       <c r="E236" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H236" t="s">
+        <v>207</v>
+      </c>
+      <c r="I236" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="C237" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H237" t="s">
+        <v>208</v>
+      </c>
+      <c r="I237" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>37</v>
       </c>
@@ -3299,32 +4001,60 @@
       <c r="C238" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A239" s="1"/>
+      <c r="I238">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A239" s="4">
+        <v>42849</v>
+      </c>
+      <c r="B239" s="5">
+        <v>0.41944444444444445</v>
+      </c>
       <c r="C239" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A240" s="1"/>
+      <c r="I239">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A240" s="4">
+        <v>42850</v>
+      </c>
+      <c r="B240" s="5">
+        <v>0.40277777777777773</v>
+      </c>
       <c r="C240" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I240">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="C241" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I241">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="C242" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H242" t="s">
+        <v>211</v>
+      </c>
+      <c r="I242" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="C243" t="s">
         <v>92</v>
@@ -3332,8 +4062,14 @@
       <c r="G243" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H243" t="s">
+        <v>212</v>
+      </c>
+      <c r="I243" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="C244" t="s">
         <v>112</v>
@@ -3341,8 +4077,14 @@
       <c r="G244" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H244" t="s">
+        <v>213</v>
+      </c>
+      <c r="I244" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="C245" t="s">
         <v>75</v>
@@ -3356,14 +4098,26 @@
       <c r="G245" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H245" t="s">
+        <v>214</v>
+      </c>
+      <c r="I245" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="C246" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H246" t="s">
+        <v>215</v>
+      </c>
+      <c r="I246" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="C247" t="s">
         <v>114</v>
@@ -3377,8 +4131,14 @@
       <c r="G247" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H247" t="s">
+        <v>216</v>
+      </c>
+      <c r="I247" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>38</v>
       </c>
@@ -3388,32 +4148,47 @@
       <c r="C248" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I248">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="C249" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I249">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="C250" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I250">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="C251" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I251">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="C252" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I252" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="C253" t="s">
         <v>98</v>
@@ -3421,14 +4196,20 @@
       <c r="G253" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H253" t="s">
+        <v>217</v>
+      </c>
+      <c r="I253" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="C254" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="C255" t="s">
         <v>111</v>
@@ -3436,8 +4217,14 @@
       <c r="G255" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H255" t="s">
+        <v>218</v>
+      </c>
+      <c r="I255" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="C256" t="s">
         <v>65</v>
@@ -3445,8 +4232,14 @@
       <c r="G256" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H256" t="s">
+        <v>219</v>
+      </c>
+      <c r="I256" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="C257" t="s">
         <v>64</v>
@@ -3454,8 +4247,14 @@
       <c r="G257" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H257" t="s">
+        <v>220</v>
+      </c>
+      <c r="I257" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="C258" t="s">
         <v>115</v>
@@ -3463,8 +4262,14 @@
       <c r="G258" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H258" t="s">
+        <v>221</v>
+      </c>
+      <c r="I258" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="C259" t="s">
         <v>116</v>
@@ -3478,8 +4283,14 @@
       <c r="G259" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H259" t="s">
+        <v>222</v>
+      </c>
+      <c r="I259" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="C260" t="s">
         <v>117</v>
@@ -3493,8 +4304,14 @@
       <c r="G260" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H260" t="s">
+        <v>222</v>
+      </c>
+      <c r="I260" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>39</v>
       </c>
@@ -3505,31 +4322,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" s="1"/>
       <c r="C262" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="C263" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="C264" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="C265" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>40</v>
       </c>
@@ -3540,67 +4357,70 @@
         <v>55</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" s="1"/>
       <c r="C267" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="C268" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="C269" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="C270" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="C271" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="C272" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="C273" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="C274" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="C275" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="C276" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I276" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>41</v>
       </c>
@@ -3610,56 +4430,71 @@
       <c r="C277" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I277">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="C278" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="C279" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="C280" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="C281" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I281">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" s="1"/>
       <c r="C282" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="C283" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" s="1"/>
       <c r="C284" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H284" t="s">
+        <v>194</v>
+      </c>
+      <c r="I284" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" s="1"/>
       <c r="C285" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I285" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" s="1"/>
       <c r="C286" t="s">
         <v>72</v>
@@ -3667,8 +4502,14 @@
       <c r="G286">
         <v>10</v>
       </c>
-    </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H286" t="s">
+        <v>223</v>
+      </c>
+      <c r="I286" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="C287" t="s">
         <v>83</v>
@@ -3679,8 +4520,14 @@
       <c r="G287" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H287" t="s">
+        <v>224</v>
+      </c>
+      <c r="I287" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>42</v>
       </c>
@@ -3693,32 +4540,44 @@
       <c r="G288">
         <v>9</v>
       </c>
-    </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H288">
+        <v>10</v>
+      </c>
+      <c r="I288">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A289" s="1"/>
       <c r="C289" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="C290" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="C291" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="C292" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H292" t="s">
+        <v>225</v>
+      </c>
+      <c r="I292" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="C293" t="s">
         <v>104</v>
@@ -3726,8 +4585,14 @@
       <c r="G293" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H293" t="s">
+        <v>218</v>
+      </c>
+      <c r="I293" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="C294" t="s">
         <v>85</v>
@@ -3735,8 +4600,14 @@
       <c r="G294" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H294" t="s">
+        <v>218</v>
+      </c>
+      <c r="I294" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="C295" t="s">
         <v>111</v>
@@ -3744,14 +4615,26 @@
       <c r="G295" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H295" t="s">
+        <v>218</v>
+      </c>
+      <c r="I295" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="C296" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H296" t="s">
+        <v>194</v>
+      </c>
+      <c r="I296" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="C297" t="s">
         <v>96</v>
@@ -3759,8 +4642,14 @@
       <c r="G297" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H297" t="s">
+        <v>218</v>
+      </c>
+      <c r="I297" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="C298" t="s">
         <v>119</v>
@@ -3768,14 +4657,26 @@
       <c r="G298" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H298" t="s">
+        <v>218</v>
+      </c>
+      <c r="I298" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="C299" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H299">
+        <v>9</v>
+      </c>
+      <c r="I299" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>43</v>
       </c>
@@ -3785,50 +4686,99 @@
       <c r="C300" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A301" s="1"/>
+      <c r="H300">
+        <v>9</v>
+      </c>
+      <c r="I300">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A301" s="4">
+        <v>42849</v>
+      </c>
+      <c r="B301" s="5">
+        <v>0.41944444444444445</v>
+      </c>
       <c r="C301" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A302" s="1"/>
+      <c r="H301">
+        <v>9</v>
+      </c>
+      <c r="I301">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A302" s="4">
+        <v>42850</v>
+      </c>
+      <c r="B302" s="5">
+        <v>0.40277777777777773</v>
+      </c>
       <c r="C302" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I302">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="C303" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I303">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="C304" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H304" t="s">
+        <v>226</v>
+      </c>
+      <c r="I304" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="C305" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H305" t="s">
+        <v>227</v>
+      </c>
+      <c r="I305" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="C306" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H306" t="s">
+        <v>228</v>
+      </c>
+      <c r="I306" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="C307" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I307" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>44</v>
       </c>
@@ -3838,56 +4788,93 @@
       <c r="C308" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A309" s="1"/>
+      <c r="I308">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A309" s="4">
+        <v>42849</v>
+      </c>
+      <c r="B309" s="5">
+        <v>0.41944444444444445</v>
+      </c>
       <c r="C309" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A310" s="1"/>
+      <c r="I309">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A310" s="4">
+        <v>42850</v>
+      </c>
+      <c r="B310" s="5">
+        <v>0.40277777777777773</v>
+      </c>
       <c r="C310" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I310">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="C311" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I311">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="C312" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I312" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="C313" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I313" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="C314" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I314">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="C315" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I315" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="C316" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I316" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>45</v>
       </c>
@@ -3897,50 +4884,59 @@
       <c r="C317" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H317">
+        <v>9</v>
+      </c>
+      <c r="I317">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="C318" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="C319" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="C320" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
       <c r="C321" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" s="1"/>
       <c r="C322" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" s="1"/>
       <c r="C323" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" s="1"/>
       <c r="C324" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I324" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>46</v>
       </c>
@@ -3951,49 +4947,64 @@
         <v>55</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" s="1"/>
       <c r="C326" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" s="1"/>
       <c r="C327" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" s="1"/>
       <c r="C328" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" s="1"/>
       <c r="C329" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I329" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="C330" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="C331" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H331" t="s">
+        <v>229</v>
+      </c>
+      <c r="I331" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="C332" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H332" t="s">
+        <v>230</v>
+      </c>
+      <c r="I332" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>47</v>
       </c>
@@ -4004,55 +5015,70 @@
         <v>55</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="C334" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A335" s="1"/>
       <c r="C335" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A336" s="1"/>
       <c r="C336" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A337" s="1"/>
       <c r="C337" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I337" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="C338" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="C339" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H339" t="s">
+        <v>204</v>
+      </c>
+      <c r="I339" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="C340" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I340" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A341" s="1"/>
       <c r="C341" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I341" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A342" s="1"/>
       <c r="C342" t="s">
         <v>133</v>
@@ -4060,26 +5086,47 @@
       <c r="G342" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H342" t="s">
+        <v>231</v>
+      </c>
+      <c r="I342" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A343" s="1"/>
       <c r="C343" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H343" t="s">
+        <v>204</v>
+      </c>
+      <c r="I343" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A344" s="1"/>
       <c r="C344" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H344" t="s">
+        <v>232</v>
+      </c>
+      <c r="I344" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A345" s="1"/>
       <c r="C345" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I345" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="C346" t="s">
         <v>122</v>
@@ -4087,8 +5134,14 @@
       <c r="G346" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H346" t="s">
+        <v>233</v>
+      </c>
+      <c r="I346" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>48</v>
       </c>
@@ -4099,31 +5152,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="C348" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
       <c r="C349" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="C350" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A351" s="1"/>
       <c r="C351" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>49</v>
       </c>
@@ -4134,43 +5187,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="C353" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="C354" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="C355" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="C356" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="C357" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="C358" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>50</v>
       </c>
@@ -4181,43 +5234,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="C360" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A361" s="1"/>
       <c r="C361" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="C362" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="C363" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="C364" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="C365" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>51</v>
       </c>
@@ -4233,33 +5286,45 @@
       <c r="G366">
         <v>9</v>
       </c>
-    </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H366">
+        <v>9</v>
+      </c>
+      <c r="I366">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C367" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C368" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C369" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="370" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C370" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C371" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="372" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="H371" t="s">
+        <v>194</v>
+      </c>
+      <c r="I371" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="372" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C372" t="s">
         <v>140</v>
       </c>

</xml_diff>